<commit_message>
[#PAB-332] Tests for upsert duplicate submission
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/Post_transform_EXAMPLE_data.xlsx
+++ b/tests/controller_tests/resources/Post_transform_EXAMPLE_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SnapeN\Dev\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC5ADD6-8865-47B0-B240-87F686718426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24853CD0-3D02-4835-BFBE-AB2E40C353C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="4725" windowWidth="28770" windowHeight="13365" firstSheet="7" activeTab="11" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
+    <workbookView xWindow="38280" yWindow="5175" windowWidth="29040" windowHeight="15720" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Ref" sheetId="20" r:id="rId1"/>
@@ -1744,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93FC7A3-FF2E-4DB3-98A7-1EC1615CB1D7}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1780,7 @@
         <v>44969</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +2097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869229C1-8ED3-40A8-834B-93A943D4A8DA}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -3385,7 +3385,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,7 +3599,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5645,7 +5645,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5699,7 +5699,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5815,7 +5815,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6649,7 +6649,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[BAU_FIX] risk register impact enums
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/Post_transform_EXAMPLE_data.xlsx
+++ b/tests/controller_tests/resources/Post_transform_EXAMPLE_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CF0F78-24BD-4FDE-A4AB-78938249F77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A6B647-D7DF-4A84-9B3F-D85FD74EBADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="2100" windowWidth="36015" windowHeight="15435" activeTab="2" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
+    <workbookView xWindow="15090" yWindow="2280" windowWidth="28140" windowHeight="17280" firstSheet="8" activeTab="15" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Ref" sheetId="20" r:id="rId1"/>
@@ -581,9 +581,6 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Mitigation 1</t>
   </si>
   <si>
-    <t>3 - Medium Impact</t>
-  </si>
-  <si>
     <t>1 - Low</t>
   </si>
   <si>
@@ -602,9 +599,6 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Mitigation 2</t>
   </si>
   <si>
-    <t>4 - Significant Impact</t>
-  </si>
-  <si>
     <t>Insufficient financial resources available to fund interventions through to completion</t>
   </si>
   <si>
@@ -617,9 +611,6 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Mitigation 3</t>
   </si>
   <si>
-    <t>5 - Major Impact</t>
-  </si>
-  <si>
     <t>4 - Close: next 3 months</t>
   </si>
   <si>
@@ -674,9 +665,6 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Mitigation 8</t>
   </si>
   <si>
-    <t>2 - Low Impact</t>
-  </si>
-  <si>
     <t>Cost and availability of materials</t>
   </si>
   <si>
@@ -743,9 +731,6 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Mitigation 15</t>
   </si>
   <si>
-    <t>1 - Marginal Impact</t>
-  </si>
-  <si>
     <t>Jane Doe- Programme Manager</t>
   </si>
   <si>
@@ -782,9 +767,6 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Mitigation 20</t>
   </si>
   <si>
-    <t>6 - Critical Impact</t>
-  </si>
-  <si>
     <t>Costs overrun</t>
   </si>
   <si>
@@ -1026,6 +1008,24 @@
   </si>
   <si>
     <t>HS</t>
+  </si>
+  <si>
+    <t>5 - Major impact</t>
+  </si>
+  <si>
+    <t>3 - Medium impact</t>
+  </si>
+  <si>
+    <t>4 - Significant impact</t>
+  </si>
+  <si>
+    <t>6 - Critical impact</t>
+  </si>
+  <si>
+    <t>2 - Low impact</t>
+  </si>
+  <si>
+    <t>1 - Marginal impact</t>
   </si>
 </sst>
 </file>
@@ -1757,16 +1757,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1921,7 +1921,7 @@
         <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2117,7 +2117,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B2" t="s">
         <v>143</v>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s">
         <v>142</v>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B6" t="s">
         <v>122</v>
@@ -2157,7 +2157,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B7" t="s">
         <v>122</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B8" t="s">
         <v>123</v>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B10" t="s">
         <v>124</v>
@@ -2189,7 +2189,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B11" t="s">
         <v>126</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B12" t="s">
         <v>126</v>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B13" t="s">
         <v>126</v>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B14" t="s">
         <v>124</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B15" t="s">
         <v>125</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B16" t="s">
         <v>125</v>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B17" t="s">
         <v>127</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B18" t="s">
         <v>127</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B19" t="s">
         <v>127</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B20" t="s">
         <v>127</v>
@@ -2334,7 +2334,7 @@
         <v>133</v>
       </c>
       <c r="H1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2348,7 +2348,7 @@
         <v>44104</v>
       </c>
       <c r="D2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E2" t="s">
         <v>134</v>
@@ -2374,7 +2374,7 @@
         <v>44286</v>
       </c>
       <c r="D3" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E3" t="s">
         <v>134</v>
@@ -2400,7 +2400,7 @@
         <v>44469</v>
       </c>
       <c r="D4" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E4" t="s">
         <v>134</v>
@@ -2426,7 +2426,7 @@
         <v>44834</v>
       </c>
       <c r="D5" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E5" t="s">
         <v>134</v>
@@ -2452,7 +2452,7 @@
         <v>45016</v>
       </c>
       <c r="D6" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E6" t="s">
         <v>134</v>
@@ -2478,7 +2478,7 @@
         <v>45199</v>
       </c>
       <c r="D7" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E7" t="s">
         <v>134</v>
@@ -2501,7 +2501,7 @@
         <v>45382</v>
       </c>
       <c r="D8" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E8" t="s">
         <v>134</v>
@@ -2524,7 +2524,7 @@
         <v>45565</v>
       </c>
       <c r="D9" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E9" t="s">
         <v>134</v>
@@ -2550,7 +2550,7 @@
         <v>45747</v>
       </c>
       <c r="D10" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E10" t="s">
         <v>134</v>
@@ -2576,7 +2576,7 @@
         <v>45930</v>
       </c>
       <c r="D11" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E11" t="s">
         <v>134</v>
@@ -2599,7 +2599,7 @@
         <v>46112</v>
       </c>
       <c r="D12" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E12" t="s">
         <v>134</v>
@@ -2875,7 +2875,7 @@
         <v>44104</v>
       </c>
       <c r="D24" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E24" t="s">
         <v>134</v>
@@ -2898,7 +2898,7 @@
         <v>44286</v>
       </c>
       <c r="D25" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E25" t="s">
         <v>134</v>
@@ -2921,7 +2921,7 @@
         <v>44469</v>
       </c>
       <c r="D26" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E26" t="s">
         <v>134</v>
@@ -2944,7 +2944,7 @@
         <v>44834</v>
       </c>
       <c r="D27" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E27" t="s">
         <v>134</v>
@@ -2967,7 +2967,7 @@
         <v>45016</v>
       </c>
       <c r="D28" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E28" t="s">
         <v>134</v>
@@ -2990,7 +2990,7 @@
         <v>45199</v>
       </c>
       <c r="D29" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E29" t="s">
         <v>134</v>
@@ -3013,7 +3013,7 @@
         <v>45382</v>
       </c>
       <c r="D30" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E30" t="s">
         <v>134</v>
@@ -3036,7 +3036,7 @@
         <v>45565</v>
       </c>
       <c r="D31" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E31" t="s">
         <v>134</v>
@@ -3059,7 +3059,7 @@
         <v>45747</v>
       </c>
       <c r="D32" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E32" t="s">
         <v>134</v>
@@ -3082,7 +3082,7 @@
         <v>45930</v>
       </c>
       <c r="D33" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E33" t="s">
         <v>134</v>
@@ -3105,7 +3105,7 @@
         <v>46112</v>
       </c>
       <c r="D34" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E34" t="s">
         <v>134</v>
@@ -3128,7 +3128,7 @@
         <v>44104</v>
       </c>
       <c r="D35" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E35" t="s">
         <v>134</v>
@@ -3151,7 +3151,7 @@
         <v>44286</v>
       </c>
       <c r="D36" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E36" t="s">
         <v>134</v>
@@ -3174,7 +3174,7 @@
         <v>44469</v>
       </c>
       <c r="D37" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E37" t="s">
         <v>134</v>
@@ -3197,7 +3197,7 @@
         <v>44834</v>
       </c>
       <c r="D38" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E38" t="s">
         <v>134</v>
@@ -3220,7 +3220,7 @@
         <v>45016</v>
       </c>
       <c r="D39" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E39" t="s">
         <v>134</v>
@@ -3243,7 +3243,7 @@
         <v>45199</v>
       </c>
       <c r="D40" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E40" t="s">
         <v>134</v>
@@ -3266,7 +3266,7 @@
         <v>45382</v>
       </c>
       <c r="D41" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E41" t="s">
         <v>134</v>
@@ -3289,7 +3289,7 @@
         <v>45565</v>
       </c>
       <c r="D42" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E42" t="s">
         <v>134</v>
@@ -3312,7 +3312,7 @@
         <v>45747</v>
       </c>
       <c r="D43" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E43" t="s">
         <v>134</v>
@@ -3335,7 +3335,7 @@
         <v>45930</v>
       </c>
       <c r="D44" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E44" t="s">
         <v>134</v>
@@ -3358,7 +3358,7 @@
         <v>46112</v>
       </c>
       <c r="D45" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E45" t="s">
         <v>134</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -3423,12 +3423,12 @@
         <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B5" t="s">
         <v>141</v>
@@ -3436,7 +3436,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -3460,7 +3460,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
@@ -3468,7 +3468,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
@@ -3476,7 +3476,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -3492,7 +3492,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B18" t="s">
         <v>140</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
@@ -3556,7 +3556,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -3564,7 +3564,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B23" t="s">
         <v>141</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B24" t="s">
         <v>141</v>
@@ -3645,7 +3645,7 @@
         <v>132</v>
       </c>
       <c r="J1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3659,7 +3659,7 @@
         <v>43951</v>
       </c>
       <c r="E2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F2" t="s">
         <v>157</v>
@@ -3674,7 +3674,7 @@
         <v>84</v>
       </c>
       <c r="J2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3688,7 +3688,7 @@
         <v>43982</v>
       </c>
       <c r="E3" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F3" t="s">
         <v>157</v>
@@ -3703,7 +3703,7 @@
         <v>84</v>
       </c>
       <c r="J3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3717,7 +3717,7 @@
         <v>44012</v>
       </c>
       <c r="E4" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F4" t="s">
         <v>157</v>
@@ -3732,7 +3732,7 @@
         <v>84</v>
       </c>
       <c r="J4" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3746,7 +3746,7 @@
         <v>44043</v>
       </c>
       <c r="E5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F5" t="s">
         <v>157</v>
@@ -3761,7 +3761,7 @@
         <v>84</v>
       </c>
       <c r="J5" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3775,7 +3775,7 @@
         <v>44074</v>
       </c>
       <c r="E6" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F6" t="s">
         <v>157</v>
@@ -3790,7 +3790,7 @@
         <v>84</v>
       </c>
       <c r="J6" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3804,7 +3804,7 @@
         <v>44104</v>
       </c>
       <c r="E7" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F7" t="s">
         <v>157</v>
@@ -3819,7 +3819,7 @@
         <v>84</v>
       </c>
       <c r="J7" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3833,7 +3833,7 @@
         <v>44135</v>
       </c>
       <c r="E8" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F8" t="s">
         <v>157</v>
@@ -3848,7 +3848,7 @@
         <v>84</v>
       </c>
       <c r="J8" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3862,7 +3862,7 @@
         <v>44165</v>
       </c>
       <c r="E9" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F9" t="s">
         <v>157</v>
@@ -3877,7 +3877,7 @@
         <v>84</v>
       </c>
       <c r="J9" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3891,7 +3891,7 @@
         <v>44196</v>
       </c>
       <c r="E10" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F10" t="s">
         <v>157</v>
@@ -3906,7 +3906,7 @@
         <v>84</v>
       </c>
       <c r="J10" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3920,7 +3920,7 @@
         <v>44227</v>
       </c>
       <c r="E11" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F11" t="s">
         <v>157</v>
@@ -3935,7 +3935,7 @@
         <v>84</v>
       </c>
       <c r="J11" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3949,7 +3949,7 @@
         <v>44255</v>
       </c>
       <c r="E12" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F12" t="s">
         <v>157</v>
@@ -3964,7 +3964,7 @@
         <v>84</v>
       </c>
       <c r="J12" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3978,7 +3978,7 @@
         <v>44286</v>
       </c>
       <c r="E13" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F13" t="s">
         <v>157</v>
@@ -3993,7 +3993,7 @@
         <v>84</v>
       </c>
       <c r="J13" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -4007,7 +4007,7 @@
         <v>44316</v>
       </c>
       <c r="E14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F14" t="s">
         <v>157</v>
@@ -4022,7 +4022,7 @@
         <v>84</v>
       </c>
       <c r="J14" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -4036,7 +4036,7 @@
         <v>44347</v>
       </c>
       <c r="E15" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F15" t="s">
         <v>157</v>
@@ -4051,7 +4051,7 @@
         <v>84</v>
       </c>
       <c r="J15" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -4065,7 +4065,7 @@
         <v>44377</v>
       </c>
       <c r="E16" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F16" t="s">
         <v>157</v>
@@ -4091,7 +4091,7 @@
         <v>44408</v>
       </c>
       <c r="E17" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F17" t="s">
         <v>157</v>
@@ -4120,10 +4120,10 @@
         <v>150</v>
       </c>
       <c r="F18" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="G18" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="H18">
         <v>28</v>
@@ -4146,10 +4146,10 @@
         <v>150</v>
       </c>
       <c r="F19" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="G19" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="H19">
         <v>33</v>
@@ -4169,7 +4169,7 @@
         <v>44500</v>
       </c>
       <c r="E20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F20" t="s">
         <v>157</v>
@@ -4195,7 +4195,7 @@
         <v>44530</v>
       </c>
       <c r="E21" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F21" t="s">
         <v>157</v>
@@ -4210,7 +4210,7 @@
         <v>84</v>
       </c>
       <c r="J21" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -4224,7 +4224,7 @@
         <v>44561</v>
       </c>
       <c r="E22" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F22" t="s">
         <v>157</v>
@@ -4239,7 +4239,7 @@
         <v>84</v>
       </c>
       <c r="J22" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
         <v>44227</v>
       </c>
       <c r="E23" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F23" t="s">
         <v>157</v>
@@ -4268,7 +4268,7 @@
         <v>84</v>
       </c>
       <c r="J23" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -4282,7 +4282,7 @@
         <v>44620</v>
       </c>
       <c r="E24" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F24" t="s">
         <v>157</v>
@@ -4297,7 +4297,7 @@
         <v>84</v>
       </c>
       <c r="J24" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
         <v>44651</v>
       </c>
       <c r="E25" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F25" t="s">
         <v>157</v>
@@ -4326,7 +4326,7 @@
         <v>84</v>
       </c>
       <c r="J25" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4343,10 +4343,10 @@
         <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="G26" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="H26">
         <v>21</v>
@@ -4355,7 +4355,7 @@
         <v>89</v>
       </c>
       <c r="J26" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -4372,10 +4372,10 @@
         <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="G27" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -4384,7 +4384,7 @@
         <v>89</v>
       </c>
       <c r="J27" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -4400,8 +4400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3428C4CB-3892-4526-BA3F-C1E2D7B4E672}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4485,7 +4485,7 @@
         <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
       <c r="I2" t="s">
         <v>174</v>
@@ -4494,16 +4494,16 @@
         <v>175</v>
       </c>
       <c r="K2" t="s">
+        <v>320</v>
+      </c>
+      <c r="L2" t="s">
         <v>176</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>177</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>178</v>
-      </c>
-      <c r="N2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -4511,10 +4511,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" t="s">
         <v>180</v>
-      </c>
-      <c r="D3" t="s">
-        <v>181</v>
       </c>
       <c r="E3" t="s">
         <v>173</v>
@@ -4526,25 +4526,25 @@
         <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="I3" t="s">
         <v>174</v>
       </c>
       <c r="J3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K3" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="L3" t="s">
+        <v>176</v>
+      </c>
+      <c r="M3" t="s">
         <v>177</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>178</v>
-      </c>
-      <c r="N3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -4552,10 +4552,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E4" t="s">
         <v>173</v>
@@ -4567,25 +4567,25 @@
         <v>98</v>
       </c>
       <c r="H4" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="I4" t="s">
+        <v>184</v>
+      </c>
+      <c r="J4" t="s">
+        <v>185</v>
+      </c>
+      <c r="K4" t="s">
+        <v>319</v>
+      </c>
+      <c r="L4" t="s">
+        <v>184</v>
+      </c>
+      <c r="M4" t="s">
         <v>186</v>
       </c>
-      <c r="J4" t="s">
-        <v>187</v>
-      </c>
-      <c r="K4" t="s">
-        <v>188</v>
-      </c>
-      <c r="L4" t="s">
-        <v>186</v>
-      </c>
-      <c r="M4" t="s">
-        <v>189</v>
-      </c>
       <c r="N4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4593,10 +4593,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E5" t="s">
         <v>173</v>
@@ -4608,25 +4608,25 @@
         <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="I5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K5" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="L5" t="s">
         <v>174</v>
       </c>
       <c r="M5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4634,10 +4634,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E6" t="s">
         <v>173</v>
@@ -4649,25 +4649,25 @@
         <v>98</v>
       </c>
       <c r="H6" t="s">
+        <v>320</v>
+      </c>
+      <c r="I6" t="s">
         <v>176</v>
       </c>
-      <c r="I6" t="s">
-        <v>177</v>
-      </c>
       <c r="J6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K6" t="s">
+        <v>320</v>
+      </c>
+      <c r="L6" t="s">
         <v>176</v>
       </c>
-      <c r="L6" t="s">
-        <v>177</v>
-      </c>
       <c r="M6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4675,10 +4675,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E7" t="s">
         <v>173</v>
@@ -4690,25 +4690,25 @@
         <v>98</v>
       </c>
       <c r="H7" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="I7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K7" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="L7" t="s">
         <v>174</v>
       </c>
       <c r="M7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4716,10 +4716,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E8" t="s">
         <v>173</v>
@@ -4731,25 +4731,25 @@
         <v>98</v>
       </c>
       <c r="H8" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="I8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K8" t="s">
+        <v>320</v>
+      </c>
+      <c r="L8" t="s">
         <v>176</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>177</v>
       </c>
-      <c r="M8" t="s">
-        <v>178</v>
-      </c>
       <c r="N8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4757,10 +4757,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E9" t="s">
         <v>173</v>
@@ -4772,25 +4772,25 @@
         <v>98</v>
       </c>
       <c r="H9" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="I9" t="s">
         <v>174</v>
       </c>
       <c r="J9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K9" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
       <c r="L9" t="s">
+        <v>176</v>
+      </c>
+      <c r="M9" t="s">
         <v>177</v>
       </c>
-      <c r="M9" t="s">
-        <v>178</v>
-      </c>
       <c r="N9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4799,10 +4799,10 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
         <v>173</v>
@@ -4814,25 +4814,25 @@
         <v>98</v>
       </c>
       <c r="H10" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="I10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K10" t="s">
+        <v>320</v>
+      </c>
+      <c r="L10" t="s">
         <v>176</v>
       </c>
-      <c r="L10" t="s">
-        <v>177</v>
-      </c>
       <c r="M10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="N10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -4841,10 +4841,10 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E11" t="s">
         <v>173</v>
@@ -4856,25 +4856,25 @@
         <v>98</v>
       </c>
       <c r="H11" t="s">
-        <v>176</v>
+        <v>320</v>
       </c>
       <c r="I11" t="s">
         <v>174</v>
       </c>
       <c r="J11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="K11" t="s">
+        <v>320</v>
+      </c>
+      <c r="L11" t="s">
         <v>176</v>
       </c>
-      <c r="L11" t="s">
-        <v>177</v>
-      </c>
       <c r="M11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N11" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -4883,10 +4883,10 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D12" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E12" t="s">
         <v>173</v>
@@ -4898,25 +4898,25 @@
         <v>98</v>
       </c>
       <c r="H12" t="s">
-        <v>176</v>
+        <v>320</v>
       </c>
       <c r="I12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J12" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K12" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
       <c r="L12" t="s">
         <v>174</v>
       </c>
       <c r="M12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N12" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -4925,10 +4925,10 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E13" t="s">
         <v>173</v>
@@ -4940,25 +4940,25 @@
         <v>98</v>
       </c>
       <c r="H13" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="I13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J13" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="K13" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="L13" t="s">
         <v>174</v>
       </c>
       <c r="M13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4967,10 +4967,10 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D14" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E14" t="s">
         <v>173</v>
@@ -4982,25 +4982,25 @@
         <v>98</v>
       </c>
       <c r="H14" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
       <c r="I14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J14" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="K14" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
       <c r="L14" t="s">
         <v>174</v>
       </c>
       <c r="M14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="N14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -5009,10 +5009,10 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D15" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E15" t="s">
         <v>173</v>
@@ -5024,25 +5024,25 @@
         <v>98</v>
       </c>
       <c r="H15" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
       <c r="I15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J15" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K15" t="s">
-        <v>176</v>
+        <v>320</v>
       </c>
       <c r="L15" t="s">
         <v>174</v>
       </c>
       <c r="M15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -5051,10 +5051,10 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E16" t="s">
         <v>173</v>
@@ -5066,25 +5066,25 @@
         <v>98</v>
       </c>
       <c r="H16" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
       <c r="I16" t="s">
+        <v>176</v>
+      </c>
+      <c r="J16" t="s">
+        <v>225</v>
+      </c>
+      <c r="K16" t="s">
+        <v>324</v>
+      </c>
+      <c r="L16" t="s">
+        <v>176</v>
+      </c>
+      <c r="M16" t="s">
         <v>177</v>
       </c>
-      <c r="J16" t="s">
-        <v>229</v>
-      </c>
-      <c r="K16" t="s">
-        <v>230</v>
-      </c>
-      <c r="L16" t="s">
-        <v>177</v>
-      </c>
-      <c r="M16" t="s">
-        <v>178</v>
-      </c>
       <c r="N16" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -5093,10 +5093,10 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D17" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E17" t="s">
         <v>173</v>
@@ -5108,25 +5108,25 @@
         <v>98</v>
       </c>
       <c r="H17" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
       <c r="I17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J17" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="K17" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="L17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M17" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -5135,10 +5135,10 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E18" t="s">
         <v>173</v>
@@ -5150,25 +5150,25 @@
         <v>98</v>
       </c>
       <c r="H18" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
       <c r="I18" t="s">
+        <v>176</v>
+      </c>
+      <c r="J18" t="s">
+        <v>230</v>
+      </c>
+      <c r="K18" t="s">
+        <v>324</v>
+      </c>
+      <c r="L18" t="s">
+        <v>176</v>
+      </c>
+      <c r="M18" t="s">
         <v>177</v>
       </c>
-      <c r="J18" t="s">
-        <v>235</v>
-      </c>
-      <c r="K18" t="s">
-        <v>230</v>
-      </c>
-      <c r="L18" t="s">
-        <v>177</v>
-      </c>
-      <c r="M18" t="s">
-        <v>178</v>
-      </c>
       <c r="N18" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -5177,10 +5177,10 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D19" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E19" t="s">
         <v>173</v>
@@ -5192,25 +5192,25 @@
         <v>98</v>
       </c>
       <c r="H19" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="I19" t="s">
         <v>174</v>
       </c>
       <c r="J19" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="K19" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
       <c r="L19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M19" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -5219,10 +5219,10 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D20" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E20" t="s">
         <v>173</v>
@@ -5234,25 +5234,25 @@
         <v>98</v>
       </c>
       <c r="H20" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
       <c r="I20" t="s">
         <v>174</v>
       </c>
       <c r="J20" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="K20" t="s">
-        <v>176</v>
+        <v>320</v>
       </c>
       <c r="L20" t="s">
         <v>174</v>
       </c>
       <c r="M20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -5261,10 +5261,10 @@
         <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D21" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E21" t="s">
         <v>173</v>
@@ -5276,25 +5276,25 @@
         <v>98</v>
       </c>
       <c r="H21" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="I21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J21" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="K21" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="L21" t="s">
         <v>174</v>
       </c>
       <c r="M21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -5303,10 +5303,10 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E22" t="s">
         <v>173</v>
@@ -5318,25 +5318,25 @@
         <v>98</v>
       </c>
       <c r="H22" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
       <c r="I22" t="s">
         <v>174</v>
       </c>
       <c r="J22" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="K22" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="L22" t="s">
         <v>174</v>
       </c>
       <c r="M22" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -5345,10 +5345,10 @@
         <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D23" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E23" t="s">
         <v>173</v>
@@ -5360,25 +5360,25 @@
         <v>98</v>
       </c>
       <c r="H23" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="I23" t="s">
         <v>174</v>
       </c>
       <c r="J23" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="K23" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="L23" t="s">
+        <v>176</v>
+      </c>
+      <c r="M23" t="s">
         <v>177</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>178</v>
-      </c>
-      <c r="N23" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -5387,10 +5387,10 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E24" t="s">
         <v>173</v>
@@ -5402,25 +5402,25 @@
         <v>98</v>
       </c>
       <c r="H24" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
       <c r="I24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J24" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="K24" t="s">
+        <v>320</v>
+      </c>
+      <c r="L24" t="s">
         <v>176</v>
       </c>
-      <c r="L24" t="s">
-        <v>177</v>
-      </c>
       <c r="M24" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="N24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -5429,10 +5429,10 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D25" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E25" t="s">
         <v>173</v>
@@ -5444,25 +5444,25 @@
         <v>98</v>
       </c>
       <c r="H25" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
       <c r="I25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J25" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="K25" t="s">
+        <v>320</v>
+      </c>
+      <c r="L25" t="s">
         <v>176</v>
       </c>
-      <c r="L25" t="s">
-        <v>177</v>
-      </c>
       <c r="M25" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -5471,10 +5471,10 @@
         <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D26" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E26" t="s">
         <v>173</v>
@@ -5486,25 +5486,25 @@
         <v>98</v>
       </c>
       <c r="H26" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="I26" t="s">
         <v>174</v>
       </c>
       <c r="J26" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="K26" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="L26" t="s">
         <v>174</v>
       </c>
       <c r="M26" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="N26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -5513,10 +5513,10 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D27" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E27" t="s">
         <v>173</v>
@@ -5528,25 +5528,25 @@
         <v>98</v>
       </c>
       <c r="H27" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
       <c r="I27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J27" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="K27" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
       <c r="L27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M27" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -5555,10 +5555,10 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E28" t="s">
         <v>173</v>
@@ -5570,25 +5570,25 @@
         <v>98</v>
       </c>
       <c r="H28" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="I28" t="s">
         <v>174</v>
       </c>
       <c r="J28" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="K28" t="s">
+        <v>320</v>
+      </c>
+      <c r="L28" t="s">
         <v>176</v>
       </c>
-      <c r="L28" t="s">
-        <v>177</v>
-      </c>
       <c r="M28" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -5644,8 +5644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136BCEBD-759D-42DA-A155-48E4E8958367}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5678,10 +5678,10 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -6393,7 +6393,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
@@ -6405,13 +6405,13 @@
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="H1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="I1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6422,7 +6422,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -6431,7 +6431,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>
@@ -6440,7 +6440,7 @@
         <v>83</v>
       </c>
       <c r="I2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -6451,7 +6451,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -6477,7 +6477,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D4" t="s">
         <v>30</v>
@@ -6489,13 +6489,13 @@
         <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="H4" t="s">
         <v>94</v>
       </c>
       <c r="I4" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6506,7 +6506,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -6532,7 +6532,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D6" t="s">
         <v>36</v>
@@ -6547,7 +6547,7 @@
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6558,7 +6558,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
@@ -6581,7 +6581,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D8" t="s">
         <v>36</v>
@@ -6599,7 +6599,7 @@
         <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -6610,7 +6610,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D9" t="s">
         <v>39</v>
@@ -6728,7 +6728,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -6784,7 +6784,7 @@
         <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -7267,6 +7267,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB5DDB95A7ECBD49AA08D06BA3EF1CDA" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95a99fb7649f76cf16eb4f5cafa7cbc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="681fe441-c46c-4ea5-a5c5-b45872725697" xmlns:ns3="6bac55d2-c587-47e2-866b-bbb6fe14d104" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbf7ff0d2c127a9a42e650b92ffbc482" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="681fe441-c46c-4ea5-a5c5-b45872725697"/>
@@ -7508,15 +7517,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7529,6 +7529,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9931E176-D5AF-4D57-88FA-0E21DE56657D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7544,14 +7552,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[BAU_FIX] impact enum trailing space fix
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/Post_transform_EXAMPLE_data.xlsx
+++ b/tests/controller_tests/resources/Post_transform_EXAMPLE_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A6B647-D7DF-4A84-9B3F-D85FD74EBADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB680991-0A45-4DDB-B545-B89022088E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15090" yWindow="2280" windowWidth="28140" windowHeight="17280" firstSheet="8" activeTab="15" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28140" windowHeight="17280" firstSheet="8" activeTab="15" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Ref" sheetId="20" r:id="rId1"/>
@@ -1010,15 +1010,9 @@
     <t>HS</t>
   </si>
   <si>
-    <t>5 - Major impact</t>
-  </si>
-  <si>
     <t>3 - Medium impact</t>
   </si>
   <si>
-    <t>4 - Significant impact</t>
-  </si>
-  <si>
     <t>6 - Critical impact</t>
   </si>
   <si>
@@ -1026,6 +1020,12 @@
   </si>
   <si>
     <t>1 - Marginal impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 - Significant impact </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 - Major impact </t>
   </si>
 </sst>
 </file>
@@ -4401,7 +4401,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4485,7 +4485,7 @@
         <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I2" t="s">
         <v>174</v>
@@ -4494,7 +4494,7 @@
         <v>175</v>
       </c>
       <c r="K2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L2" t="s">
         <v>176</v>
@@ -4526,7 +4526,7 @@
         <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I3" t="s">
         <v>174</v>
@@ -4535,7 +4535,7 @@
         <v>181</v>
       </c>
       <c r="K3" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="L3" t="s">
         <v>176</v>
@@ -4567,7 +4567,7 @@
         <v>98</v>
       </c>
       <c r="H4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I4" t="s">
         <v>184</v>
@@ -4576,7 +4576,7 @@
         <v>185</v>
       </c>
       <c r="K4" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="L4" t="s">
         <v>184</v>
@@ -4608,7 +4608,7 @@
         <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I5" t="s">
         <v>184</v>
@@ -4617,7 +4617,7 @@
         <v>189</v>
       </c>
       <c r="K5" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="L5" t="s">
         <v>174</v>
@@ -4649,7 +4649,7 @@
         <v>98</v>
       </c>
       <c r="H6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I6" t="s">
         <v>176</v>
@@ -4658,7 +4658,7 @@
         <v>192</v>
       </c>
       <c r="K6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L6" t="s">
         <v>176</v>
@@ -4690,7 +4690,7 @@
         <v>98</v>
       </c>
       <c r="H7" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I7" t="s">
         <v>184</v>
@@ -4699,7 +4699,7 @@
         <v>195</v>
       </c>
       <c r="K7" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="L7" t="s">
         <v>174</v>
@@ -4731,7 +4731,7 @@
         <v>98</v>
       </c>
       <c r="H8" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I8" t="s">
         <v>184</v>
@@ -4740,7 +4740,7 @@
         <v>199</v>
       </c>
       <c r="K8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L8" t="s">
         <v>176</v>
@@ -4772,7 +4772,7 @@
         <v>98</v>
       </c>
       <c r="H9" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I9" t="s">
         <v>174</v>
@@ -4781,7 +4781,7 @@
         <v>203</v>
       </c>
       <c r="K9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L9" t="s">
         <v>176</v>
@@ -4814,7 +4814,7 @@
         <v>98</v>
       </c>
       <c r="H10" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I10" t="s">
         <v>184</v>
@@ -4823,7 +4823,7 @@
         <v>205</v>
       </c>
       <c r="K10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L10" t="s">
         <v>176</v>
@@ -4856,7 +4856,7 @@
         <v>98</v>
       </c>
       <c r="H11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I11" t="s">
         <v>174</v>
@@ -4865,7 +4865,7 @@
         <v>210</v>
       </c>
       <c r="K11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L11" t="s">
         <v>176</v>
@@ -4898,7 +4898,7 @@
         <v>98</v>
       </c>
       <c r="H12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I12" t="s">
         <v>184</v>
@@ -4907,7 +4907,7 @@
         <v>214</v>
       </c>
       <c r="K12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L12" t="s">
         <v>174</v>
@@ -4940,7 +4940,7 @@
         <v>98</v>
       </c>
       <c r="H13" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I13" t="s">
         <v>184</v>
@@ -4949,7 +4949,7 @@
         <v>217</v>
       </c>
       <c r="K13" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="L13" t="s">
         <v>174</v>
@@ -4982,7 +4982,7 @@
         <v>98</v>
       </c>
       <c r="H14" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I14" t="s">
         <v>184</v>
@@ -4991,7 +4991,7 @@
         <v>220</v>
       </c>
       <c r="K14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L14" t="s">
         <v>174</v>
@@ -5024,7 +5024,7 @@
         <v>98</v>
       </c>
       <c r="H15" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I15" t="s">
         <v>184</v>
@@ -5033,7 +5033,7 @@
         <v>223</v>
       </c>
       <c r="K15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L15" t="s">
         <v>174</v>
@@ -5066,7 +5066,7 @@
         <v>98</v>
       </c>
       <c r="H16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I16" t="s">
         <v>176</v>
@@ -5075,7 +5075,7 @@
         <v>225</v>
       </c>
       <c r="K16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L16" t="s">
         <v>176</v>
@@ -5108,7 +5108,7 @@
         <v>98</v>
       </c>
       <c r="H17" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I17" t="s">
         <v>176</v>
@@ -5117,7 +5117,7 @@
         <v>228</v>
       </c>
       <c r="K17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L17" t="s">
         <v>176</v>
@@ -5150,7 +5150,7 @@
         <v>98</v>
       </c>
       <c r="H18" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I18" t="s">
         <v>176</v>
@@ -5159,7 +5159,7 @@
         <v>230</v>
       </c>
       <c r="K18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L18" t="s">
         <v>176</v>
@@ -5192,7 +5192,7 @@
         <v>98</v>
       </c>
       <c r="H19" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I19" t="s">
         <v>174</v>
@@ -5201,7 +5201,7 @@
         <v>233</v>
       </c>
       <c r="K19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L19" t="s">
         <v>176</v>
@@ -5234,7 +5234,7 @@
         <v>98</v>
       </c>
       <c r="H20" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I20" t="s">
         <v>174</v>
@@ -5243,7 +5243,7 @@
         <v>235</v>
       </c>
       <c r="K20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L20" t="s">
         <v>174</v>
@@ -5276,7 +5276,7 @@
         <v>98</v>
       </c>
       <c r="H21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I21" t="s">
         <v>184</v>
@@ -5285,7 +5285,7 @@
         <v>237</v>
       </c>
       <c r="K21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="L21" t="s">
         <v>174</v>
@@ -5318,7 +5318,7 @@
         <v>98</v>
       </c>
       <c r="H22" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I22" t="s">
         <v>174</v>
@@ -5327,7 +5327,7 @@
         <v>239</v>
       </c>
       <c r="K22" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="L22" t="s">
         <v>174</v>
@@ -5360,7 +5360,7 @@
         <v>98</v>
       </c>
       <c r="H23" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I23" t="s">
         <v>174</v>
@@ -5369,7 +5369,7 @@
         <v>242</v>
       </c>
       <c r="K23" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="L23" t="s">
         <v>176</v>
@@ -5402,7 +5402,7 @@
         <v>98</v>
       </c>
       <c r="H24" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I24" t="s">
         <v>176</v>
@@ -5411,7 +5411,7 @@
         <v>244</v>
       </c>
       <c r="K24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L24" t="s">
         <v>176</v>
@@ -5444,7 +5444,7 @@
         <v>98</v>
       </c>
       <c r="H25" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I25" t="s">
         <v>176</v>
@@ -5453,7 +5453,7 @@
         <v>247</v>
       </c>
       <c r="K25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L25" t="s">
         <v>176</v>
@@ -5486,7 +5486,7 @@
         <v>98</v>
       </c>
       <c r="H26" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I26" t="s">
         <v>174</v>
@@ -5495,7 +5495,7 @@
         <v>250</v>
       </c>
       <c r="K26" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="L26" t="s">
         <v>174</v>
@@ -5528,7 +5528,7 @@
         <v>98</v>
       </c>
       <c r="H27" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I27" t="s">
         <v>176</v>
@@ -5537,7 +5537,7 @@
         <v>254</v>
       </c>
       <c r="K27" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L27" t="s">
         <v>176</v>
@@ -5570,7 +5570,7 @@
         <v>98</v>
       </c>
       <c r="H28" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I28" t="s">
         <v>174</v>
@@ -5579,7 +5579,7 @@
         <v>256</v>
       </c>
       <c r="K28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L28" t="s">
         <v>176</v>
@@ -7267,15 +7267,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB5DDB95A7ECBD49AA08D06BA3EF1CDA" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95a99fb7649f76cf16eb4f5cafa7cbc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="681fe441-c46c-4ea5-a5c5-b45872725697" xmlns:ns3="6bac55d2-c587-47e2-866b-bbb6fe14d104" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbf7ff0d2c127a9a42e650b92ffbc482" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="681fe441-c46c-4ea5-a5c5-b45872725697"/>
@@ -7517,7 +7508,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="681fe441-c46c-4ea5-a5c5-b45872725697">
@@ -7528,15 +7519,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9931E176-D5AF-4D57-88FA-0E21DE56657D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7556,7 +7548,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70073AC4-B26C-493C-8C25-29DBD67F7B7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7567,6 +7559,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{95c71a0f-75e1-4c8f-90e2-641c9351dd98}" enabled="1" method="Standard" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" removed="0"/>

</xml_diff>

<commit_message>
[BAU_FIX] align marginal impact enum with submission enum
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/Post_transform_EXAMPLE_data.xlsx
+++ b/tests/controller_tests/resources/Post_transform_EXAMPLE_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB680991-0A45-4DDB-B545-B89022088E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9518FE4-FABB-4B72-B03D-120720AF0FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28140" windowHeight="17280" firstSheet="8" activeTab="15" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" firstSheet="8" activeTab="15" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Ref" sheetId="20" r:id="rId1"/>
@@ -1019,13 +1019,13 @@
     <t>2 - Low impact</t>
   </si>
   <si>
-    <t>1 - Marginal impact</t>
-  </si>
-  <si>
     <t xml:space="preserve">4 - Significant impact </t>
   </si>
   <si>
     <t xml:space="preserve">5 - Major impact </t>
+  </si>
+  <si>
+    <t>1- Marginal impact</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1037,7 @@
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1748,14 +1748,14 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>257</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>16508</v>
       </c>
@@ -1796,13 +1796,13 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1894,7 +1894,7 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
@@ -1904,7 +1904,7 @@
     <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2101,13 +2101,13 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="93.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>283</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>284</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>285</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>286</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>287</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>288</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>289</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>290</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>291</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>292</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>293</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>294</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>295</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>296</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>297</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>298</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>299</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>300</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>301</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="20" t="s">
         <v>135</v>
       </c>
@@ -2299,7 +2299,7 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -2311,7 +2311,7 @@
     <col min="8" max="8" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -3388,13 +3388,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="101.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>137</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>302</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>304</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>305</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>147</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>306</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>307</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>308</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>309</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>150</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>151</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>152</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>310</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>153</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>311</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>312</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>313</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>314</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>315</v>
       </c>
@@ -3602,7 +3602,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -3616,7 +3616,7 @@
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="B22" t="s">
         <v>3</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="B25" t="s">
         <v>3</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="13.5" customHeight="1">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -4401,10 +4401,10 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -4421,7 +4421,7 @@
     <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I2" t="s">
         <v>174</v>
@@ -4506,7 +4506,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I3" t="s">
         <v>174</v>
@@ -4535,7 +4535,7 @@
         <v>181</v>
       </c>
       <c r="K3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L3" t="s">
         <v>176</v>
@@ -4547,7 +4547,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>185</v>
       </c>
       <c r="K4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L4" t="s">
         <v>184</v>
@@ -4588,7 +4588,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I5" t="s">
         <v>184</v>
@@ -4617,7 +4617,7 @@
         <v>189</v>
       </c>
       <c r="K5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L5" t="s">
         <v>174</v>
@@ -4629,7 +4629,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>98</v>
       </c>
       <c r="H7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I7" t="s">
         <v>184</v>
@@ -4699,7 +4699,7 @@
         <v>195</v>
       </c>
       <c r="K7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L7" t="s">
         <v>174</v>
@@ -4711,7 +4711,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>98</v>
       </c>
       <c r="H8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I8" t="s">
         <v>184</v>
@@ -4752,7 +4752,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>98</v>
       </c>
       <c r="H9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I9" t="s">
         <v>174</v>
@@ -4793,7 +4793,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>27</v>
@@ -4814,7 +4814,7 @@
         <v>98</v>
       </c>
       <c r="H10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I10" t="s">
         <v>184</v>
@@ -4835,7 +4835,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
         <v>27</v>
@@ -4877,7 +4877,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>27</v>
@@ -4919,7 +4919,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>29</v>
@@ -4949,7 +4949,7 @@
         <v>217</v>
       </c>
       <c r="K13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L13" t="s">
         <v>174</v>
@@ -4961,7 +4961,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
         <v>29</v>
@@ -4982,7 +4982,7 @@
         <v>98</v>
       </c>
       <c r="H14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I14" t="s">
         <v>184</v>
@@ -5003,7 +5003,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>29</v>
@@ -5024,7 +5024,7 @@
         <v>98</v>
       </c>
       <c r="H15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I15" t="s">
         <v>184</v>
@@ -5045,7 +5045,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
         <v>33</v>
@@ -5075,7 +5075,7 @@
         <v>225</v>
       </c>
       <c r="K16" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="L16" t="s">
         <v>176</v>
@@ -5087,7 +5087,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
         <v>33</v>
@@ -5117,7 +5117,7 @@
         <v>228</v>
       </c>
       <c r="K17" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="L17" t="s">
         <v>176</v>
@@ -5129,7 +5129,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>33</v>
@@ -5159,7 +5159,7 @@
         <v>230</v>
       </c>
       <c r="K18" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="L18" t="s">
         <v>176</v>
@@ -5171,7 +5171,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
         <v>35</v>
@@ -5192,7 +5192,7 @@
         <v>98</v>
       </c>
       <c r="H19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I19" t="s">
         <v>174</v>
@@ -5213,7 +5213,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
         <v>35</v>
@@ -5234,7 +5234,7 @@
         <v>98</v>
       </c>
       <c r="H20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I20" t="s">
         <v>174</v>
@@ -5255,7 +5255,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
         <v>35</v>
@@ -5297,7 +5297,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
         <v>35</v>
@@ -5318,7 +5318,7 @@
         <v>98</v>
       </c>
       <c r="H22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I22" t="s">
         <v>174</v>
@@ -5327,7 +5327,7 @@
         <v>239</v>
       </c>
       <c r="K22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L22" t="s">
         <v>174</v>
@@ -5339,7 +5339,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
         <v>35</v>
@@ -5360,7 +5360,7 @@
         <v>98</v>
       </c>
       <c r="H23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I23" t="s">
         <v>174</v>
@@ -5369,7 +5369,7 @@
         <v>242</v>
       </c>
       <c r="K23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L23" t="s">
         <v>176</v>
@@ -5381,7 +5381,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
         <v>35</v>
@@ -5402,7 +5402,7 @@
         <v>98</v>
       </c>
       <c r="H24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I24" t="s">
         <v>176</v>
@@ -5423,7 +5423,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
         <v>35</v>
@@ -5444,7 +5444,7 @@
         <v>98</v>
       </c>
       <c r="H25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I25" t="s">
         <v>176</v>
@@ -5465,7 +5465,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
         <v>35</v>
@@ -5495,7 +5495,7 @@
         <v>250</v>
       </c>
       <c r="K26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L26" t="s">
         <v>174</v>
@@ -5507,7 +5507,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
         <v>35</v>
@@ -5528,7 +5528,7 @@
         <v>98</v>
       </c>
       <c r="H27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I27" t="s">
         <v>176</v>
@@ -5549,7 +5549,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
         <v>35</v>
@@ -5570,7 +5570,7 @@
         <v>98</v>
       </c>
       <c r="H28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I28" t="s">
         <v>174</v>
@@ -5609,13 +5609,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>271</v>
       </c>
@@ -5648,7 +5648,7 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
@@ -5656,7 +5656,7 @@
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5702,14 +5702,14 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="113.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -5818,7 +5818,7 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
@@ -5826,7 +5826,7 @@
     <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -6073,7 +6073,7 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="82" bestFit="1" customWidth="1"/>
@@ -6082,7 +6082,7 @@
     <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -6342,7 +6342,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -6373,7 +6373,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.28515625" customWidth="1"/>
@@ -6385,7 +6385,7 @@
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -6524,7 +6524,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6628,10 +6628,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="B15" s="3"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4">
       <c r="D21" s="6"/>
     </row>
   </sheetData>
@@ -6652,7 +6652,7 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -6667,7 +6667,7 @@
     <col min="11" max="11" width="63.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -6731,7 +6731,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -6758,7 +6758,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -6787,12 +6787,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="K6" s="1"/>
@@ -6818,7 +6818,7 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
@@ -6830,7 +6830,7 @@
     <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="14" t="s">
         <v>27</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="16" t="s">
         <v>27</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="14" t="s">
         <v>27</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="16" t="s">
         <v>27</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="14" t="s">
         <v>27</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="16" t="s">
         <v>27</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="14" t="s">
         <v>27</v>
       </c>
@@ -7064,7 +7064,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="16" t="s">
         <v>27</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="14" t="s">
         <v>27</v>
       </c>
@@ -7116,7 +7116,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="16" t="s">
         <v>27</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="16" t="s">
         <v>27</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="14" t="s">
         <v>27</v>
       </c>
@@ -7220,36 +7220,36 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8">
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8">
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8">
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8">
       <c r="B20" s="13"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8">
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8">
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8">
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
     </row>
@@ -7509,6 +7509,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="681fe441-c46c-4ea5-a5c5-b45872725697">
@@ -7517,15 +7526,6 @@
     <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7549,6 +7549,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70073AC4-B26C-493C-8C25-29DBD67F7B7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7559,14 +7567,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{95c71a0f-75e1-4c8f-90e2-641c9351dd98}" enabled="1" method="Standard" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" removed="0"/>

</xml_diff>